<commit_message>
Aggiunta rinse03 del 20/04/2020
</commit_message>
<xml_diff>
--- a/esercizi.xlsx
+++ b/esercizi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gieck\Documents\GitHub\iomimuovoacasa.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\GitHub\iomimuovoacasa.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D00160-EDD0-4767-85D5-C8511621D42C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E42884E-2FB3-458A-B14E-2778E3066867}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10380" xr2:uid="{D04ACDA4-7515-4249-AF43-4A86ACDA9557}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D04ACDA4-7515-4249-AF43-4A86ACDA9557}"/>
   </bookViews>
   <sheets>
     <sheet name="esercizi" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="369">
   <si>
     <t>cartella</t>
   </si>
@@ -1140,6 +1140,12 @@
   </si>
   <si>
     <t>Materiale: una palla e un birillo Numero giocatori: almeno 2 (un cavaliere e un soldato)</t>
+  </si>
+  <si>
+    <t>rinse03.mp4</t>
+  </si>
+  <si>
+    <t>rinse03</t>
   </si>
 </sst>
 </file>
@@ -1505,16 +1511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F28B5828-1DD9-429E-936D-554BBAB67831}">
   <dimension ref="A1:AF327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="123" workbookViewId="0">
-      <selection activeCell="D2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="123" workbookViewId="0">
+      <selection activeCell="D174" sqref="D174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.54296875" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="32.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="32.54296875" style="1"/>
+    <col min="1" max="16384" width="32.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1564,7 +1570,7 @@
       <c r="AE1" s="2"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" ht="147.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:32" ht="165" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1620,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" ht="191.75" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:32" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1670,7 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" ht="177" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:32" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1714,7 +1720,7 @@
       <c r="AE4" s="2"/>
       <c r="AF4" s="2"/>
     </row>
-    <row r="5" spans="1:32" ht="250.75" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:32" ht="285" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1764,7 +1770,7 @@
       <c r="AE5" s="2"/>
       <c r="AF5" s="2"/>
     </row>
-    <row r="6" spans="1:32" ht="103.25" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:32" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1814,7 +1820,7 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:32" ht="177" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:32" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1864,7 +1870,7 @@
       <c r="AE7" s="2"/>
       <c r="AF7" s="2"/>
     </row>
-    <row r="8" spans="1:32" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:32" ht="180" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1914,7 +1920,7 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
     </row>
-    <row r="9" spans="1:32" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:32" ht="240" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1964,7 +1970,7 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32" ht="309.75" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:32" ht="330" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -2014,7 +2020,7 @@
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
     </row>
-    <row r="11" spans="1:32" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:32" ht="240" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -2064,7 +2070,7 @@
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
     </row>
-    <row r="12" spans="1:32" ht="177" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:32" ht="195" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2114,7 +2120,7 @@
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
     </row>
-    <row r="13" spans="1:32" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:32" ht="180" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -2164,7 +2170,7 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:32" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:32" ht="165" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -2214,7 +2220,7 @@
       <c r="AE14" s="2"/>
       <c r="AF14" s="2"/>
     </row>
-    <row r="15" spans="1:32" ht="191.75" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:32" ht="225" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +2270,7 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:32" ht="162.25" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:32" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -2314,7 +2320,7 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
     </row>
-    <row r="17" spans="1:32" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:32" ht="240" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -2364,7 +2370,7 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="1:32" ht="309.75" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:32" ht="330" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -2414,7 +2420,7 @@
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
     </row>
-    <row r="19" spans="1:32" ht="206.5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:32" ht="240" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -2464,7 +2470,7 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>142</v>
       </c>
@@ -2508,7 +2514,7 @@
       <c r="AE20" s="2"/>
       <c r="AF20" s="2"/>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>142</v>
       </c>
@@ -2552,7 +2558,7 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>142</v>
       </c>
@@ -2596,7 +2602,7 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>142</v>
       </c>
@@ -2640,7 +2646,7 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>142</v>
       </c>
@@ -2684,7 +2690,7 @@
       <c r="AE24" s="2"/>
       <c r="AF24" s="2"/>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>142</v>
       </c>
@@ -2728,7 +2734,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>142</v>
       </c>
@@ -2772,7 +2778,7 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>142</v>
       </c>
@@ -2816,7 +2822,7 @@
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>142</v>
       </c>
@@ -2860,7 +2866,7 @@
       <c r="AE28" s="2"/>
       <c r="AF28" s="2"/>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>142</v>
       </c>
@@ -2904,7 +2910,7 @@
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>142</v>
       </c>
@@ -2948,7 +2954,7 @@
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>142</v>
       </c>
@@ -2992,7 +2998,7 @@
       <c r="AE31" s="2"/>
       <c r="AF31" s="2"/>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>142</v>
       </c>
@@ -3036,7 +3042,7 @@
       <c r="AE32" s="2"/>
       <c r="AF32" s="2"/>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>142</v>
       </c>
@@ -3080,7 +3086,7 @@
       <c r="AE33" s="2"/>
       <c r="AF33" s="2"/>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>142</v>
       </c>
@@ -3124,7 +3130,7 @@
       <c r="AE34" s="2"/>
       <c r="AF34" s="2"/>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>142</v>
       </c>
@@ -3168,7 +3174,7 @@
       <c r="AE35" s="2"/>
       <c r="AF35" s="2"/>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>142</v>
       </c>
@@ -3212,7 +3218,7 @@
       <c r="AE36" s="2"/>
       <c r="AF36" s="2"/>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>142</v>
       </c>
@@ -3256,7 +3262,7 @@
       <c r="AE37" s="2"/>
       <c r="AF37" s="2"/>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>142</v>
       </c>
@@ -3300,7 +3306,7 @@
       <c r="AE38" s="2"/>
       <c r="AF38" s="2"/>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>142</v>
       </c>
@@ -3344,7 +3350,7 @@
       <c r="AE39" s="2"/>
       <c r="AF39" s="2"/>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>142</v>
       </c>
@@ -3388,7 +3394,7 @@
       <c r="AE40" s="2"/>
       <c r="AF40" s="2"/>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>142</v>
       </c>
@@ -3432,7 +3438,7 @@
       <c r="AE41" s="2"/>
       <c r="AF41" s="2"/>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>142</v>
       </c>
@@ -3476,7 +3482,7 @@
       <c r="AE42" s="2"/>
       <c r="AF42" s="2"/>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>142</v>
       </c>
@@ -3520,7 +3526,7 @@
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>142</v>
       </c>
@@ -3564,7 +3570,7 @@
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>142</v>
       </c>
@@ -3608,7 +3614,7 @@
       <c r="AE45" s="2"/>
       <c r="AF45" s="2"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>142</v>
       </c>
@@ -3652,7 +3658,7 @@
       <c r="AE46" s="2"/>
       <c r="AF46" s="2"/>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>142</v>
       </c>
@@ -3696,7 +3702,7 @@
       <c r="AE47" s="2"/>
       <c r="AF47" s="2"/>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
@@ -3740,7 +3746,7 @@
       <c r="AE48" s="2"/>
       <c r="AF48" s="2"/>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>142</v>
       </c>
@@ -3784,7 +3790,7 @@
       <c r="AE49" s="2"/>
       <c r="AF49" s="2"/>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>142</v>
       </c>
@@ -3828,7 +3834,7 @@
       <c r="AE50" s="2"/>
       <c r="AF50" s="2"/>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>142</v>
       </c>
@@ -3872,7 +3878,7 @@
       <c r="AE51" s="2"/>
       <c r="AF51" s="2"/>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>142</v>
       </c>
@@ -3916,7 +3922,7 @@
       <c r="AE52" s="2"/>
       <c r="AF52" s="2"/>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>142</v>
       </c>
@@ -3960,7 +3966,7 @@
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>142</v>
       </c>
@@ -4004,7 +4010,7 @@
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>142</v>
       </c>
@@ -4048,7 +4054,7 @@
       <c r="AE55" s="2"/>
       <c r="AF55" s="2"/>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>142</v>
       </c>
@@ -4092,7 +4098,7 @@
       <c r="AE56" s="2"/>
       <c r="AF56" s="2"/>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>142</v>
       </c>
@@ -4136,7 +4142,7 @@
       <c r="AE57" s="2"/>
       <c r="AF57" s="2"/>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>142</v>
       </c>
@@ -4180,7 +4186,7 @@
       <c r="AE58" s="2"/>
       <c r="AF58" s="2"/>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>142</v>
       </c>
@@ -4224,7 +4230,7 @@
       <c r="AE59" s="2"/>
       <c r="AF59" s="2"/>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>142</v>
       </c>
@@ -4268,7 +4274,7 @@
       <c r="AE60" s="2"/>
       <c r="AF60" s="2"/>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>142</v>
       </c>
@@ -4312,7 +4318,7 @@
       <c r="AE61" s="2"/>
       <c r="AF61" s="2"/>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>142</v>
       </c>
@@ -4356,7 +4362,7 @@
       <c r="AE62" s="2"/>
       <c r="AF62" s="2"/>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>142</v>
       </c>
@@ -4400,7 +4406,7 @@
       <c r="AE63" s="2"/>
       <c r="AF63" s="2"/>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>142</v>
       </c>
@@ -4444,7 +4450,7 @@
       <c r="AE64" s="2"/>
       <c r="AF64" s="2"/>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>142</v>
       </c>
@@ -4488,7 +4494,7 @@
       <c r="AE65" s="2"/>
       <c r="AF65" s="2"/>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>142</v>
       </c>
@@ -4532,7 +4538,7 @@
       <c r="AE66" s="2"/>
       <c r="AF66" s="2"/>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>142</v>
       </c>
@@ -4576,7 +4582,7 @@
       <c r="AE67" s="2"/>
       <c r="AF67" s="2"/>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>142</v>
       </c>
@@ -4620,7 +4626,7 @@
       <c r="AE68" s="2"/>
       <c r="AF68" s="2"/>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>142</v>
       </c>
@@ -4664,7 +4670,7 @@
       <c r="AE69" s="2"/>
       <c r="AF69" s="2"/>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>142</v>
       </c>
@@ -4708,7 +4714,7 @@
       <c r="AE70" s="2"/>
       <c r="AF70" s="2"/>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>142</v>
       </c>
@@ -4752,7 +4758,7 @@
       <c r="AE71" s="2"/>
       <c r="AF71" s="2"/>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>142</v>
       </c>
@@ -4796,7 +4802,7 @@
       <c r="AE72" s="2"/>
       <c r="AF72" s="2"/>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>142</v>
       </c>
@@ -4840,7 +4846,7 @@
       <c r="AE73" s="2"/>
       <c r="AF73" s="2"/>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>142</v>
       </c>
@@ -4884,7 +4890,7 @@
       <c r="AE74" s="2"/>
       <c r="AF74" s="2"/>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>142</v>
       </c>
@@ -4928,7 +4934,7 @@
       <c r="AE75" s="2"/>
       <c r="AF75" s="2"/>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>142</v>
       </c>
@@ -4972,7 +4978,7 @@
       <c r="AE76" s="2"/>
       <c r="AF76" s="2"/>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>142</v>
       </c>
@@ -5016,7 +5022,7 @@
       <c r="AE77" s="2"/>
       <c r="AF77" s="2"/>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>142</v>
       </c>
@@ -5060,7 +5066,7 @@
       <c r="AE78" s="2"/>
       <c r="AF78" s="2"/>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>142</v>
       </c>
@@ -5104,7 +5110,7 @@
       <c r="AE79" s="2"/>
       <c r="AF79" s="2"/>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>142</v>
       </c>
@@ -5148,7 +5154,7 @@
       <c r="AE80" s="2"/>
       <c r="AF80" s="2"/>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>142</v>
       </c>
@@ -5192,7 +5198,7 @@
       <c r="AE81" s="2"/>
       <c r="AF81" s="2"/>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>142</v>
       </c>
@@ -5236,7 +5242,7 @@
       <c r="AE82" s="2"/>
       <c r="AF82" s="2"/>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>142</v>
       </c>
@@ -5280,7 +5286,7 @@
       <c r="AE83" s="2"/>
       <c r="AF83" s="2"/>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>142</v>
       </c>
@@ -5324,7 +5330,7 @@
       <c r="AE84" s="2"/>
       <c r="AF84" s="2"/>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>143</v>
       </c>
@@ -5368,7 +5374,7 @@
       <c r="AE85" s="2"/>
       <c r="AF85" s="2"/>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>143</v>
       </c>
@@ -5412,7 +5418,7 @@
       <c r="AE86" s="2"/>
       <c r="AF86" s="2"/>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>143</v>
       </c>
@@ -5456,7 +5462,7 @@
       <c r="AE87" s="2"/>
       <c r="AF87" s="2"/>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>143</v>
       </c>
@@ -5500,7 +5506,7 @@
       <c r="AE88" s="2"/>
       <c r="AF88" s="2"/>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>143</v>
       </c>
@@ -5544,7 +5550,7 @@
       <c r="AE89" s="2"/>
       <c r="AF89" s="2"/>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>143</v>
       </c>
@@ -5588,7 +5594,7 @@
       <c r="AE90" s="2"/>
       <c r="AF90" s="2"/>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -5632,7 +5638,7 @@
       <c r="AE91" s="2"/>
       <c r="AF91" s="2"/>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>143</v>
       </c>
@@ -5676,7 +5682,7 @@
       <c r="AE92" s="2"/>
       <c r="AF92" s="2"/>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>143</v>
       </c>
@@ -5720,7 +5726,7 @@
       <c r="AE93" s="2"/>
       <c r="AF93" s="2"/>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>142</v>
       </c>
@@ -5764,7 +5770,7 @@
       <c r="AE94" s="2"/>
       <c r="AF94" s="2"/>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>142</v>
       </c>
@@ -5808,7 +5814,7 @@
       <c r="AE95" s="2"/>
       <c r="AF95" s="2"/>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>142</v>
       </c>
@@ -5852,7 +5858,7 @@
       <c r="AE96" s="2"/>
       <c r="AF96" s="2"/>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>142</v>
       </c>
@@ -5896,7 +5902,7 @@
       <c r="AE97" s="2"/>
       <c r="AF97" s="2"/>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>142</v>
       </c>
@@ -5940,7 +5946,7 @@
       <c r="AE98" s="2"/>
       <c r="AF98" s="2"/>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>142</v>
       </c>
@@ -5984,7 +5990,7 @@
       <c r="AE99" s="2"/>
       <c r="AF99" s="2"/>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>142</v>
       </c>
@@ -6028,7 +6034,7 @@
       <c r="AE100" s="2"/>
       <c r="AF100" s="2"/>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>142</v>
       </c>
@@ -6072,7 +6078,7 @@
       <c r="AE101" s="2"/>
       <c r="AF101" s="2"/>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>142</v>
       </c>
@@ -6116,7 +6122,7 @@
       <c r="AE102" s="2"/>
       <c r="AF102" s="2"/>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>142</v>
       </c>
@@ -6160,7 +6166,7 @@
       <c r="AE103" s="2"/>
       <c r="AF103" s="2"/>
     </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>142</v>
       </c>
@@ -6204,7 +6210,7 @@
       <c r="AE104" s="2"/>
       <c r="AF104" s="2"/>
     </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>142</v>
       </c>
@@ -6248,7 +6254,7 @@
       <c r="AE105" s="2"/>
       <c r="AF105" s="2"/>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>142</v>
       </c>
@@ -6292,7 +6298,7 @@
       <c r="AE106" s="2"/>
       <c r="AF106" s="2"/>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>142</v>
       </c>
@@ -6336,7 +6342,7 @@
       <c r="AE107" s="2"/>
       <c r="AF107" s="2"/>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>3</v>
       </c>
@@ -6380,7 +6386,7 @@
       <c r="AE108" s="2"/>
       <c r="AF108" s="2"/>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>3</v>
       </c>
@@ -6424,7 +6430,7 @@
       <c r="AE109" s="2"/>
       <c r="AF109" s="2"/>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>3</v>
       </c>
@@ -6468,7 +6474,7 @@
       <c r="AE110" s="2"/>
       <c r="AF110" s="2"/>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>3</v>
       </c>
@@ -6512,7 +6518,7 @@
       <c r="AE111" s="2"/>
       <c r="AF111" s="2"/>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>3</v>
       </c>
@@ -6556,7 +6562,7 @@
       <c r="AE112" s="2"/>
       <c r="AF112" s="2"/>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>3</v>
       </c>
@@ -6600,7 +6606,7 @@
       <c r="AE113" s="2"/>
       <c r="AF113" s="2"/>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>3</v>
       </c>
@@ -6644,7 +6650,7 @@
       <c r="AE114" s="2"/>
       <c r="AF114" s="2"/>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>3</v>
       </c>
@@ -6688,7 +6694,7 @@
       <c r="AE115" s="2"/>
       <c r="AF115" s="2"/>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>3</v>
       </c>
@@ -6732,7 +6738,7 @@
       <c r="AE116" s="2"/>
       <c r="AF116" s="2"/>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>3</v>
       </c>
@@ -6776,7 +6782,7 @@
       <c r="AE117" s="2"/>
       <c r="AF117" s="2"/>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>3</v>
       </c>
@@ -6820,7 +6826,7 @@
       <c r="AE118" s="2"/>
       <c r="AF118" s="2"/>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>3</v>
       </c>
@@ -6864,7 +6870,7 @@
       <c r="AE119" s="2"/>
       <c r="AF119" s="2"/>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>3</v>
       </c>
@@ -6908,7 +6914,7 @@
       <c r="AE120" s="2"/>
       <c r="AF120" s="2"/>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>3</v>
       </c>
@@ -6952,7 +6958,7 @@
       <c r="AE121" s="2"/>
       <c r="AF121" s="2"/>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>3</v>
       </c>
@@ -6996,7 +7002,7 @@
       <c r="AE122" s="2"/>
       <c r="AF122" s="2"/>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>3</v>
       </c>
@@ -7040,7 +7046,7 @@
       <c r="AE123" s="2"/>
       <c r="AF123" s="2"/>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>3</v>
       </c>
@@ -7084,7 +7090,7 @@
       <c r="AE124" s="2"/>
       <c r="AF124" s="2"/>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>3</v>
       </c>
@@ -7128,7 +7134,7 @@
       <c r="AE125" s="2"/>
       <c r="AF125" s="2"/>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>3</v>
       </c>
@@ -7172,7 +7178,7 @@
       <c r="AE126" s="2"/>
       <c r="AF126" s="2"/>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>3</v>
       </c>
@@ -7216,7 +7222,7 @@
       <c r="AE127" s="2"/>
       <c r="AF127" s="2"/>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>3</v>
       </c>
@@ -7260,7 +7266,7 @@
       <c r="AE128" s="2"/>
       <c r="AF128" s="2"/>
     </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>3</v>
       </c>
@@ -7304,7 +7310,7 @@
       <c r="AE129" s="2"/>
       <c r="AF129" s="2"/>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>272</v>
       </c>
@@ -7348,7 +7354,7 @@
       <c r="AE130" s="2"/>
       <c r="AF130" s="2"/>
     </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>272</v>
       </c>
@@ -7392,7 +7398,7 @@
       <c r="AE131" s="2"/>
       <c r="AF131" s="2"/>
     </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>272</v>
       </c>
@@ -7436,7 +7442,7 @@
       <c r="AE132" s="2"/>
       <c r="AF132" s="2"/>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>272</v>
       </c>
@@ -7480,7 +7486,7 @@
       <c r="AE133" s="2"/>
       <c r="AF133" s="2"/>
     </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>272</v>
       </c>
@@ -7524,7 +7530,7 @@
       <c r="AE134" s="2"/>
       <c r="AF134" s="2"/>
     </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>272</v>
       </c>
@@ -7568,7 +7574,7 @@
       <c r="AE135" s="2"/>
       <c r="AF135" s="2"/>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>272</v>
       </c>
@@ -7612,7 +7618,7 @@
       <c r="AE136" s="2"/>
       <c r="AF136" s="2"/>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>272</v>
       </c>
@@ -7656,7 +7662,7 @@
       <c r="AE137" s="2"/>
       <c r="AF137" s="2"/>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>272</v>
       </c>
@@ -7700,7 +7706,7 @@
       <c r="AE138" s="2"/>
       <c r="AF138" s="2"/>
     </row>
-    <row r="139" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>272</v>
       </c>
@@ -7744,7 +7750,7 @@
       <c r="AE139" s="2"/>
       <c r="AF139" s="2"/>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>272</v>
       </c>
@@ -7788,7 +7794,7 @@
       <c r="AE140" s="2"/>
       <c r="AF140" s="2"/>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>272</v>
       </c>
@@ -7832,7 +7838,7 @@
       <c r="AE141" s="2"/>
       <c r="AF141" s="2"/>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>272</v>
       </c>
@@ -7876,7 +7882,7 @@
       <c r="AE142" s="2"/>
       <c r="AF142" s="2"/>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>272</v>
       </c>
@@ -7920,7 +7926,7 @@
       <c r="AE143" s="2"/>
       <c r="AF143" s="2"/>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>272</v>
       </c>
@@ -7964,7 +7970,7 @@
       <c r="AE144" s="2"/>
       <c r="AF144" s="2"/>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>272</v>
       </c>
@@ -8008,7 +8014,7 @@
       <c r="AE145" s="2"/>
       <c r="AF145" s="2"/>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>272</v>
       </c>
@@ -8052,7 +8058,7 @@
       <c r="AE146" s="2"/>
       <c r="AF146" s="2"/>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>272</v>
       </c>
@@ -8096,7 +8102,7 @@
       <c r="AE147" s="2"/>
       <c r="AF147" s="2"/>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>272</v>
       </c>
@@ -8140,7 +8146,7 @@
       <c r="AE148" s="2"/>
       <c r="AF148" s="2"/>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>272</v>
       </c>
@@ -8184,7 +8190,7 @@
       <c r="AE149" s="2"/>
       <c r="AF149" s="2"/>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>272</v>
       </c>
@@ -8228,7 +8234,7 @@
       <c r="AE150" s="2"/>
       <c r="AF150" s="2"/>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>272</v>
       </c>
@@ -8272,7 +8278,7 @@
       <c r="AE151" s="2"/>
       <c r="AF151" s="2"/>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>272</v>
       </c>
@@ -8316,7 +8322,7 @@
       <c r="AE152" s="2"/>
       <c r="AF152" s="2"/>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>272</v>
       </c>
@@ -8360,7 +8366,7 @@
       <c r="AE153" s="2"/>
       <c r="AF153" s="2"/>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>272</v>
       </c>
@@ -8404,7 +8410,7 @@
       <c r="AE154" s="2"/>
       <c r="AF154" s="2"/>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>272</v>
       </c>
@@ -8448,7 +8454,7 @@
       <c r="AE155" s="2"/>
       <c r="AF155" s="2"/>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>272</v>
       </c>
@@ -8492,7 +8498,7 @@
       <c r="AE156" s="2"/>
       <c r="AF156" s="2"/>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -8536,7 +8542,7 @@
       <c r="AE157" s="2"/>
       <c r="AF157" s="2"/>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>272</v>
       </c>
@@ -8580,7 +8586,7 @@
       <c r="AE158" s="2"/>
       <c r="AF158" s="2"/>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>272</v>
       </c>
@@ -8624,7 +8630,7 @@
       <c r="AE159" s="2"/>
       <c r="AF159" s="2"/>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>272</v>
       </c>
@@ -8668,7 +8674,7 @@
       <c r="AE160" s="2"/>
       <c r="AF160" s="2"/>
     </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>272</v>
       </c>
@@ -8712,7 +8718,7 @@
       <c r="AE161" s="2"/>
       <c r="AF161" s="2"/>
     </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>272</v>
       </c>
@@ -8756,7 +8762,7 @@
       <c r="AE162" s="2"/>
       <c r="AF162" s="2"/>
     </row>
-    <row r="163" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>272</v>
       </c>
@@ -8800,7 +8806,7 @@
       <c r="AE163" s="2"/>
       <c r="AF163" s="2"/>
     </row>
-    <row r="164" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>272</v>
       </c>
@@ -8844,7 +8850,7 @@
       <c r="AE164" s="2"/>
       <c r="AF164" s="2"/>
     </row>
-    <row r="165" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>272</v>
       </c>
@@ -8888,7 +8894,7 @@
       <c r="AE165" s="2"/>
       <c r="AF165" s="2"/>
     </row>
-    <row r="166" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>272</v>
       </c>
@@ -8932,7 +8938,7 @@
       <c r="AE166" s="2"/>
       <c r="AF166" s="2"/>
     </row>
-    <row r="167" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>272</v>
       </c>
@@ -8976,7 +8982,7 @@
       <c r="AE167" s="2"/>
       <c r="AF167" s="2"/>
     </row>
-    <row r="168" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>272</v>
       </c>
@@ -9020,7 +9026,7 @@
       <c r="AE168" s="2"/>
       <c r="AF168" s="2"/>
     </row>
-    <row r="169" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>272</v>
       </c>
@@ -9064,7 +9070,7 @@
       <c r="AE169" s="2"/>
       <c r="AF169" s="2"/>
     </row>
-    <row r="170" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>272</v>
       </c>
@@ -9108,7 +9114,7 @@
       <c r="AE170" s="2"/>
       <c r="AF170" s="2"/>
     </row>
-    <row r="171" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>272</v>
       </c>
@@ -9152,7 +9158,7 @@
       <c r="AE171" s="2"/>
       <c r="AF171" s="2"/>
     </row>
-    <row r="172" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>272</v>
       </c>
@@ -9196,7 +9202,7 @@
       <c r="AE172" s="2"/>
       <c r="AF172" s="2"/>
     </row>
-    <row r="173" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>272</v>
       </c>
@@ -9240,12 +9246,22 @@
       <c r="AE173" s="2"/>
       <c r="AF173" s="2"/>
     </row>
-    <row r="174" spans="1:32" x14ac:dyDescent="0.75">
-      <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="2"/>
+    <row r="174" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F174" s="2"/>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -9274,7 +9290,7 @@
       <c r="AE174" s="2"/>
       <c r="AF174" s="2"/>
     </row>
-    <row r="175" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -9308,7 +9324,7 @@
       <c r="AE175" s="2"/>
       <c r="AF175" s="2"/>
     </row>
-    <row r="176" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -9342,7 +9358,7 @@
       <c r="AE176" s="2"/>
       <c r="AF176" s="2"/>
     </row>
-    <row r="177" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -9376,7 +9392,7 @@
       <c r="AE177" s="2"/>
       <c r="AF177" s="2"/>
     </row>
-    <row r="178" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -9410,7 +9426,7 @@
       <c r="AE178" s="2"/>
       <c r="AF178" s="2"/>
     </row>
-    <row r="179" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -9444,7 +9460,7 @@
       <c r="AE179" s="2"/>
       <c r="AF179" s="2"/>
     </row>
-    <row r="180" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -9478,7 +9494,7 @@
       <c r="AE180" s="2"/>
       <c r="AF180" s="2"/>
     </row>
-    <row r="181" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -9512,7 +9528,7 @@
       <c r="AE181" s="2"/>
       <c r="AF181" s="2"/>
     </row>
-    <row r="182" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -9546,7 +9562,7 @@
       <c r="AE182" s="2"/>
       <c r="AF182" s="2"/>
     </row>
-    <row r="183" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -9580,7 +9596,7 @@
       <c r="AE183" s="2"/>
       <c r="AF183" s="2"/>
     </row>
-    <row r="184" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -9614,7 +9630,7 @@
       <c r="AE184" s="2"/>
       <c r="AF184" s="2"/>
     </row>
-    <row r="185" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -9648,7 +9664,7 @@
       <c r="AE185" s="2"/>
       <c r="AF185" s="2"/>
     </row>
-    <row r="186" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -9682,7 +9698,7 @@
       <c r="AE186" s="2"/>
       <c r="AF186" s="2"/>
     </row>
-    <row r="187" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -9716,7 +9732,7 @@
       <c r="AE187" s="2"/>
       <c r="AF187" s="2"/>
     </row>
-    <row r="188" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -9750,7 +9766,7 @@
       <c r="AE188" s="2"/>
       <c r="AF188" s="2"/>
     </row>
-    <row r="189" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="189" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -9784,7 +9800,7 @@
       <c r="AE189" s="2"/>
       <c r="AF189" s="2"/>
     </row>
-    <row r="190" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="190" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -9818,7 +9834,7 @@
       <c r="AE190" s="2"/>
       <c r="AF190" s="2"/>
     </row>
-    <row r="191" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="191" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -9852,7 +9868,7 @@
       <c r="AE191" s="2"/>
       <c r="AF191" s="2"/>
     </row>
-    <row r="192" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -9886,7 +9902,7 @@
       <c r="AE192" s="2"/>
       <c r="AF192" s="2"/>
     </row>
-    <row r="193" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="193" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -9920,7 +9936,7 @@
       <c r="AE193" s="2"/>
       <c r="AF193" s="2"/>
     </row>
-    <row r="194" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="194" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -9954,7 +9970,7 @@
       <c r="AE194" s="2"/>
       <c r="AF194" s="2"/>
     </row>
-    <row r="195" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="195" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -9988,7 +10004,7 @@
       <c r="AE195" s="2"/>
       <c r="AF195" s="2"/>
     </row>
-    <row r="196" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="196" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -10022,7 +10038,7 @@
       <c r="AE196" s="2"/>
       <c r="AF196" s="2"/>
     </row>
-    <row r="197" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="197" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -10056,7 +10072,7 @@
       <c r="AE197" s="2"/>
       <c r="AF197" s="2"/>
     </row>
-    <row r="198" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="198" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -10090,7 +10106,7 @@
       <c r="AE198" s="2"/>
       <c r="AF198" s="2"/>
     </row>
-    <row r="199" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="199" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -10124,7 +10140,7 @@
       <c r="AE199" s="2"/>
       <c r="AF199" s="2"/>
     </row>
-    <row r="200" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="200" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -10158,7 +10174,7 @@
       <c r="AE200" s="2"/>
       <c r="AF200" s="2"/>
     </row>
-    <row r="201" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="201" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -10192,7 +10208,7 @@
       <c r="AE201" s="2"/>
       <c r="AF201" s="2"/>
     </row>
-    <row r="202" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="202" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -10226,7 +10242,7 @@
       <c r="AE202" s="2"/>
       <c r="AF202" s="2"/>
     </row>
-    <row r="203" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="203" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -10260,7 +10276,7 @@
       <c r="AE203" s="2"/>
       <c r="AF203" s="2"/>
     </row>
-    <row r="204" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="204" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -10294,7 +10310,7 @@
       <c r="AE204" s="2"/>
       <c r="AF204" s="2"/>
     </row>
-    <row r="205" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="205" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -10328,7 +10344,7 @@
       <c r="AE205" s="2"/>
       <c r="AF205" s="2"/>
     </row>
-    <row r="206" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="206" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -10362,7 +10378,7 @@
       <c r="AE206" s="2"/>
       <c r="AF206" s="2"/>
     </row>
-    <row r="207" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="207" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -10396,7 +10412,7 @@
       <c r="AE207" s="2"/>
       <c r="AF207" s="2"/>
     </row>
-    <row r="208" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="208" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -10430,7 +10446,7 @@
       <c r="AE208" s="2"/>
       <c r="AF208" s="2"/>
     </row>
-    <row r="209" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="209" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -10464,7 +10480,7 @@
       <c r="AE209" s="2"/>
       <c r="AF209" s="2"/>
     </row>
-    <row r="210" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="210" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -10498,7 +10514,7 @@
       <c r="AE210" s="2"/>
       <c r="AF210" s="2"/>
     </row>
-    <row r="211" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="211" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -10532,7 +10548,7 @@
       <c r="AE211" s="2"/>
       <c r="AF211" s="2"/>
     </row>
-    <row r="212" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="212" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -10566,7 +10582,7 @@
       <c r="AE212" s="2"/>
       <c r="AF212" s="2"/>
     </row>
-    <row r="213" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="213" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -10600,7 +10616,7 @@
       <c r="AE213" s="2"/>
       <c r="AF213" s="2"/>
     </row>
-    <row r="214" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="214" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -10634,7 +10650,7 @@
       <c r="AE214" s="2"/>
       <c r="AF214" s="2"/>
     </row>
-    <row r="215" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="215" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -10668,7 +10684,7 @@
       <c r="AE215" s="2"/>
       <c r="AF215" s="2"/>
     </row>
-    <row r="216" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="216" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -10702,7 +10718,7 @@
       <c r="AE216" s="2"/>
       <c r="AF216" s="2"/>
     </row>
-    <row r="217" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="217" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -10736,7 +10752,7 @@
       <c r="AE217" s="2"/>
       <c r="AF217" s="2"/>
     </row>
-    <row r="218" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="218" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -10770,7 +10786,7 @@
       <c r="AE218" s="2"/>
       <c r="AF218" s="2"/>
     </row>
-    <row r="219" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="219" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -10804,7 +10820,7 @@
       <c r="AE219" s="2"/>
       <c r="AF219" s="2"/>
     </row>
-    <row r="220" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="220" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -10838,7 +10854,7 @@
       <c r="AE220" s="2"/>
       <c r="AF220" s="2"/>
     </row>
-    <row r="221" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="221" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -10872,7 +10888,7 @@
       <c r="AE221" s="2"/>
       <c r="AF221" s="2"/>
     </row>
-    <row r="222" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="222" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -10906,7 +10922,7 @@
       <c r="AE222" s="2"/>
       <c r="AF222" s="2"/>
     </row>
-    <row r="223" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="223" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
@@ -10940,7 +10956,7 @@
       <c r="AE223" s="2"/>
       <c r="AF223" s="2"/>
     </row>
-    <row r="224" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="224" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -10974,7 +10990,7 @@
       <c r="AE224" s="2"/>
       <c r="AF224" s="2"/>
     </row>
-    <row r="225" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="225" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
@@ -11008,7 +11024,7 @@
       <c r="AE225" s="2"/>
       <c r="AF225" s="2"/>
     </row>
-    <row r="226" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="226" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
@@ -11042,7 +11058,7 @@
       <c r="AE226" s="2"/>
       <c r="AF226" s="2"/>
     </row>
-    <row r="227" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="227" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -11076,7 +11092,7 @@
       <c r="AE227" s="2"/>
       <c r="AF227" s="2"/>
     </row>
-    <row r="228" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="228" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -11110,7 +11126,7 @@
       <c r="AE228" s="2"/>
       <c r="AF228" s="2"/>
     </row>
-    <row r="229" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="229" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A229" s="2"/>
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
@@ -11144,7 +11160,7 @@
       <c r="AE229" s="2"/>
       <c r="AF229" s="2"/>
     </row>
-    <row r="230" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="230" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
@@ -11178,7 +11194,7 @@
       <c r="AE230" s="2"/>
       <c r="AF230" s="2"/>
     </row>
-    <row r="231" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="231" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A231" s="2"/>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
@@ -11212,7 +11228,7 @@
       <c r="AE231" s="2"/>
       <c r="AF231" s="2"/>
     </row>
-    <row r="232" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="232" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A232" s="2"/>
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
@@ -11246,7 +11262,7 @@
       <c r="AE232" s="2"/>
       <c r="AF232" s="2"/>
     </row>
-    <row r="233" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="233" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A233" s="2"/>
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
@@ -11280,7 +11296,7 @@
       <c r="AE233" s="2"/>
       <c r="AF233" s="2"/>
     </row>
-    <row r="234" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="234" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A234" s="2"/>
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
@@ -11314,7 +11330,7 @@
       <c r="AE234" s="2"/>
       <c r="AF234" s="2"/>
     </row>
-    <row r="235" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="235" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A235" s="2"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
@@ -11348,7 +11364,7 @@
       <c r="AE235" s="2"/>
       <c r="AF235" s="2"/>
     </row>
-    <row r="236" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="236" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
@@ -11382,7 +11398,7 @@
       <c r="AE236" s="2"/>
       <c r="AF236" s="2"/>
     </row>
-    <row r="237" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="237" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A237" s="2"/>
       <c r="B237" s="2"/>
       <c r="C237" s="2"/>
@@ -11416,7 +11432,7 @@
       <c r="AE237" s="2"/>
       <c r="AF237" s="2"/>
     </row>
-    <row r="238" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="238" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A238" s="2"/>
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
@@ -11450,7 +11466,7 @@
       <c r="AE238" s="2"/>
       <c r="AF238" s="2"/>
     </row>
-    <row r="239" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="239" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A239" s="2"/>
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
@@ -11484,7 +11500,7 @@
       <c r="AE239" s="2"/>
       <c r="AF239" s="2"/>
     </row>
-    <row r="240" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="240" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A240" s="2"/>
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
@@ -11518,7 +11534,7 @@
       <c r="AE240" s="2"/>
       <c r="AF240" s="2"/>
     </row>
-    <row r="241" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="241" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A241" s="2"/>
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
@@ -11552,7 +11568,7 @@
       <c r="AE241" s="2"/>
       <c r="AF241" s="2"/>
     </row>
-    <row r="242" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="242" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A242" s="2"/>
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
@@ -11586,7 +11602,7 @@
       <c r="AE242" s="2"/>
       <c r="AF242" s="2"/>
     </row>
-    <row r="243" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="243" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A243" s="2"/>
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
@@ -11620,7 +11636,7 @@
       <c r="AE243" s="2"/>
       <c r="AF243" s="2"/>
     </row>
-    <row r="244" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="244" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
@@ -11654,7 +11670,7 @@
       <c r="AE244" s="2"/>
       <c r="AF244" s="2"/>
     </row>
-    <row r="245" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="245" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A245" s="2"/>
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
@@ -11688,7 +11704,7 @@
       <c r="AE245" s="2"/>
       <c r="AF245" s="2"/>
     </row>
-    <row r="246" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="246" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
@@ -11722,7 +11738,7 @@
       <c r="AE246" s="2"/>
       <c r="AF246" s="2"/>
     </row>
-    <row r="247" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="247" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A247" s="2"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
@@ -11756,7 +11772,7 @@
       <c r="AE247" s="2"/>
       <c r="AF247" s="2"/>
     </row>
-    <row r="248" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="248" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A248" s="2"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -11790,7 +11806,7 @@
       <c r="AE248" s="2"/>
       <c r="AF248" s="2"/>
     </row>
-    <row r="249" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="249" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A249" s="2"/>
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
@@ -11824,7 +11840,7 @@
       <c r="AE249" s="2"/>
       <c r="AF249" s="2"/>
     </row>
-    <row r="250" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="250" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A250" s="2"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -11858,7 +11874,7 @@
       <c r="AE250" s="2"/>
       <c r="AF250" s="2"/>
     </row>
-    <row r="251" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A251" s="2"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
@@ -11892,7 +11908,7 @@
       <c r="AE251" s="2"/>
       <c r="AF251" s="2"/>
     </row>
-    <row r="252" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="252" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A252" s="2"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -11926,7 +11942,7 @@
       <c r="AE252" s="2"/>
       <c r="AF252" s="2"/>
     </row>
-    <row r="253" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="253" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A253" s="2"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
@@ -11960,7 +11976,7 @@
       <c r="AE253" s="2"/>
       <c r="AF253" s="2"/>
     </row>
-    <row r="254" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="254" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A254" s="2"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -11994,7 +12010,7 @@
       <c r="AE254" s="2"/>
       <c r="AF254" s="2"/>
     </row>
-    <row r="255" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="255" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A255" s="2"/>
       <c r="B255" s="2"/>
       <c r="C255" s="2"/>
@@ -12028,7 +12044,7 @@
       <c r="AE255" s="2"/>
       <c r="AF255" s="2"/>
     </row>
-    <row r="256" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="256" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A256" s="2"/>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -12062,7 +12078,7 @@
       <c r="AE256" s="2"/>
       <c r="AF256" s="2"/>
     </row>
-    <row r="257" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="257" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A257" s="2"/>
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
@@ -12096,7 +12112,7 @@
       <c r="AE257" s="2"/>
       <c r="AF257" s="2"/>
     </row>
-    <row r="258" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="258" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A258" s="2"/>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -12130,7 +12146,7 @@
       <c r="AE258" s="2"/>
       <c r="AF258" s="2"/>
     </row>
-    <row r="259" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="259" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A259" s="2"/>
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
@@ -12164,7 +12180,7 @@
       <c r="AE259" s="2"/>
       <c r="AF259" s="2"/>
     </row>
-    <row r="260" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="260" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A260" s="2"/>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -12198,7 +12214,7 @@
       <c r="AE260" s="2"/>
       <c r="AF260" s="2"/>
     </row>
-    <row r="261" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="261" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A261" s="2"/>
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
@@ -12232,7 +12248,7 @@
       <c r="AE261" s="2"/>
       <c r="AF261" s="2"/>
     </row>
-    <row r="262" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="262" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
@@ -12266,7 +12282,7 @@
       <c r="AE262" s="2"/>
       <c r="AF262" s="2"/>
     </row>
-    <row r="263" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="263" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A263" s="2"/>
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
@@ -12300,7 +12316,7 @@
       <c r="AE263" s="2"/>
       <c r="AF263" s="2"/>
     </row>
-    <row r="264" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="264" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A264" s="2"/>
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
@@ -12334,7 +12350,7 @@
       <c r="AE264" s="2"/>
       <c r="AF264" s="2"/>
     </row>
-    <row r="265" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="265" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A265" s="2"/>
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
@@ -12368,7 +12384,7 @@
       <c r="AE265" s="2"/>
       <c r="AF265" s="2"/>
     </row>
-    <row r="266" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="266" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A266" s="2"/>
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
@@ -12402,7 +12418,7 @@
       <c r="AE266" s="2"/>
       <c r="AF266" s="2"/>
     </row>
-    <row r="267" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="267" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A267" s="2"/>
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
@@ -12436,7 +12452,7 @@
       <c r="AE267" s="2"/>
       <c r="AF267" s="2"/>
     </row>
-    <row r="268" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="268" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A268" s="2"/>
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
@@ -12470,7 +12486,7 @@
       <c r="AE268" s="2"/>
       <c r="AF268" s="2"/>
     </row>
-    <row r="269" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="269" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A269" s="2"/>
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
@@ -12504,7 +12520,7 @@
       <c r="AE269" s="2"/>
       <c r="AF269" s="2"/>
     </row>
-    <row r="270" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="270" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A270" s="2"/>
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
@@ -12538,7 +12554,7 @@
       <c r="AE270" s="2"/>
       <c r="AF270" s="2"/>
     </row>
-    <row r="271" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="271" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A271" s="2"/>
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
@@ -12572,7 +12588,7 @@
       <c r="AE271" s="2"/>
       <c r="AF271" s="2"/>
     </row>
-    <row r="272" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="272" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A272" s="2"/>
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
@@ -12606,7 +12622,7 @@
       <c r="AE272" s="2"/>
       <c r="AF272" s="2"/>
     </row>
-    <row r="273" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="273" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A273" s="2"/>
       <c r="B273" s="2"/>
       <c r="C273" s="2"/>
@@ -12640,7 +12656,7 @@
       <c r="AE273" s="2"/>
       <c r="AF273" s="2"/>
     </row>
-    <row r="274" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="274" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A274" s="2"/>
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
@@ -12674,7 +12690,7 @@
       <c r="AE274" s="2"/>
       <c r="AF274" s="2"/>
     </row>
-    <row r="275" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="275" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A275" s="2"/>
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
@@ -12708,7 +12724,7 @@
       <c r="AE275" s="2"/>
       <c r="AF275" s="2"/>
     </row>
-    <row r="276" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="276" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A276" s="2"/>
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
@@ -12742,7 +12758,7 @@
       <c r="AE276" s="2"/>
       <c r="AF276" s="2"/>
     </row>
-    <row r="277" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="277" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A277" s="2"/>
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
@@ -12776,7 +12792,7 @@
       <c r="AE277" s="2"/>
       <c r="AF277" s="2"/>
     </row>
-    <row r="278" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="278" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A278" s="2"/>
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
@@ -12810,7 +12826,7 @@
       <c r="AE278" s="2"/>
       <c r="AF278" s="2"/>
     </row>
-    <row r="279" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="279" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A279" s="2"/>
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
@@ -12844,7 +12860,7 @@
       <c r="AE279" s="2"/>
       <c r="AF279" s="2"/>
     </row>
-    <row r="280" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="280" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A280" s="2"/>
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
@@ -12878,7 +12894,7 @@
       <c r="AE280" s="2"/>
       <c r="AF280" s="2"/>
     </row>
-    <row r="281" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="281" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A281" s="2"/>
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
@@ -12912,7 +12928,7 @@
       <c r="AE281" s="2"/>
       <c r="AF281" s="2"/>
     </row>
-    <row r="282" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="282" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A282" s="2"/>
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
@@ -12946,7 +12962,7 @@
       <c r="AE282" s="2"/>
       <c r="AF282" s="2"/>
     </row>
-    <row r="283" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="283" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A283" s="2"/>
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
@@ -12980,7 +12996,7 @@
       <c r="AE283" s="2"/>
       <c r="AF283" s="2"/>
     </row>
-    <row r="284" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="284" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A284" s="2"/>
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
@@ -13014,7 +13030,7 @@
       <c r="AE284" s="2"/>
       <c r="AF284" s="2"/>
     </row>
-    <row r="285" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="285" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A285" s="2"/>
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
@@ -13048,7 +13064,7 @@
       <c r="AE285" s="2"/>
       <c r="AF285" s="2"/>
     </row>
-    <row r="286" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="286" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A286" s="2"/>
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
@@ -13082,7 +13098,7 @@
       <c r="AE286" s="2"/>
       <c r="AF286" s="2"/>
     </row>
-    <row r="287" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="287" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A287" s="2"/>
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
@@ -13116,7 +13132,7 @@
       <c r="AE287" s="2"/>
       <c r="AF287" s="2"/>
     </row>
-    <row r="288" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="288" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A288" s="2"/>
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
@@ -13150,7 +13166,7 @@
       <c r="AE288" s="2"/>
       <c r="AF288" s="2"/>
     </row>
-    <row r="289" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="289" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A289" s="2"/>
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
@@ -13184,7 +13200,7 @@
       <c r="AE289" s="2"/>
       <c r="AF289" s="2"/>
     </row>
-    <row r="290" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="290" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A290" s="2"/>
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
@@ -13218,7 +13234,7 @@
       <c r="AE290" s="2"/>
       <c r="AF290" s="2"/>
     </row>
-    <row r="291" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="291" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A291" s="2"/>
       <c r="B291" s="2"/>
       <c r="C291" s="2"/>
@@ -13252,7 +13268,7 @@
       <c r="AE291" s="2"/>
       <c r="AF291" s="2"/>
     </row>
-    <row r="292" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="292" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A292" s="2"/>
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
@@ -13286,7 +13302,7 @@
       <c r="AE292" s="2"/>
       <c r="AF292" s="2"/>
     </row>
-    <row r="293" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="293" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A293" s="2"/>
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
@@ -13320,7 +13336,7 @@
       <c r="AE293" s="2"/>
       <c r="AF293" s="2"/>
     </row>
-    <row r="294" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="294" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A294" s="2"/>
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
@@ -13354,7 +13370,7 @@
       <c r="AE294" s="2"/>
       <c r="AF294" s="2"/>
     </row>
-    <row r="295" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="295" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A295" s="2"/>
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
@@ -13388,7 +13404,7 @@
       <c r="AE295" s="2"/>
       <c r="AF295" s="2"/>
     </row>
-    <row r="296" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="296" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A296" s="2"/>
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
@@ -13422,7 +13438,7 @@
       <c r="AE296" s="2"/>
       <c r="AF296" s="2"/>
     </row>
-    <row r="297" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="297" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A297" s="2"/>
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
@@ -13456,7 +13472,7 @@
       <c r="AE297" s="2"/>
       <c r="AF297" s="2"/>
     </row>
-    <row r="298" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="298" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A298" s="2"/>
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
@@ -13490,7 +13506,7 @@
       <c r="AE298" s="2"/>
       <c r="AF298" s="2"/>
     </row>
-    <row r="299" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="299" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A299" s="2"/>
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
@@ -13524,7 +13540,7 @@
       <c r="AE299" s="2"/>
       <c r="AF299" s="2"/>
     </row>
-    <row r="300" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="300" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A300" s="2"/>
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
@@ -13558,7 +13574,7 @@
       <c r="AE300" s="2"/>
       <c r="AF300" s="2"/>
     </row>
-    <row r="301" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="301" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A301" s="2"/>
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
@@ -13592,7 +13608,7 @@
       <c r="AE301" s="2"/>
       <c r="AF301" s="2"/>
     </row>
-    <row r="302" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="302" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A302" s="2"/>
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
@@ -13626,7 +13642,7 @@
       <c r="AE302" s="2"/>
       <c r="AF302" s="2"/>
     </row>
-    <row r="303" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="303" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A303" s="2"/>
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
@@ -13660,7 +13676,7 @@
       <c r="AE303" s="2"/>
       <c r="AF303" s="2"/>
     </row>
-    <row r="304" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="304" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A304" s="2"/>
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
@@ -13694,7 +13710,7 @@
       <c r="AE304" s="2"/>
       <c r="AF304" s="2"/>
     </row>
-    <row r="305" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="305" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A305" s="2"/>
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
@@ -13728,7 +13744,7 @@
       <c r="AE305" s="2"/>
       <c r="AF305" s="2"/>
     </row>
-    <row r="306" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="306" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A306" s="2"/>
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
@@ -13762,7 +13778,7 @@
       <c r="AE306" s="2"/>
       <c r="AF306" s="2"/>
     </row>
-    <row r="307" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="307" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A307" s="2"/>
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
@@ -13796,7 +13812,7 @@
       <c r="AE307" s="2"/>
       <c r="AF307" s="2"/>
     </row>
-    <row r="308" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="308" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A308" s="2"/>
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
@@ -13830,7 +13846,7 @@
       <c r="AE308" s="2"/>
       <c r="AF308" s="2"/>
     </row>
-    <row r="309" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="309" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A309" s="2"/>
       <c r="B309" s="2"/>
       <c r="C309" s="2"/>
@@ -13864,7 +13880,7 @@
       <c r="AE309" s="2"/>
       <c r="AF309" s="2"/>
     </row>
-    <row r="310" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="310" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A310" s="2"/>
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
@@ -13898,7 +13914,7 @@
       <c r="AE310" s="2"/>
       <c r="AF310" s="2"/>
     </row>
-    <row r="311" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="311" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A311" s="2"/>
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
@@ -13932,7 +13948,7 @@
       <c r="AE311" s="2"/>
       <c r="AF311" s="2"/>
     </row>
-    <row r="312" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="312" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A312" s="2"/>
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
@@ -13966,7 +13982,7 @@
       <c r="AE312" s="2"/>
       <c r="AF312" s="2"/>
     </row>
-    <row r="313" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="313" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A313" s="2"/>
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
@@ -14000,7 +14016,7 @@
       <c r="AE313" s="2"/>
       <c r="AF313" s="2"/>
     </row>
-    <row r="314" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="314" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A314" s="2"/>
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
@@ -14034,7 +14050,7 @@
       <c r="AE314" s="2"/>
       <c r="AF314" s="2"/>
     </row>
-    <row r="315" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="315" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A315" s="2"/>
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
@@ -14068,7 +14084,7 @@
       <c r="AE315" s="2"/>
       <c r="AF315" s="2"/>
     </row>
-    <row r="316" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="316" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A316" s="2"/>
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
@@ -14102,7 +14118,7 @@
       <c r="AE316" s="2"/>
       <c r="AF316" s="2"/>
     </row>
-    <row r="317" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="317" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A317" s="2"/>
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
@@ -14136,7 +14152,7 @@
       <c r="AE317" s="2"/>
       <c r="AF317" s="2"/>
     </row>
-    <row r="318" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="318" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A318" s="2"/>
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
@@ -14170,7 +14186,7 @@
       <c r="AE318" s="2"/>
       <c r="AF318" s="2"/>
     </row>
-    <row r="319" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="319" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A319" s="2"/>
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
@@ -14204,7 +14220,7 @@
       <c r="AE319" s="2"/>
       <c r="AF319" s="2"/>
     </row>
-    <row r="320" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="320" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A320" s="2"/>
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
@@ -14238,7 +14254,7 @@
       <c r="AE320" s="2"/>
       <c r="AF320" s="2"/>
     </row>
-    <row r="321" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="321" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A321" s="2"/>
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
@@ -14272,7 +14288,7 @@
       <c r="AE321" s="2"/>
       <c r="AF321" s="2"/>
     </row>
-    <row r="322" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="322" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A322" s="2"/>
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
@@ -14306,7 +14322,7 @@
       <c r="AE322" s="2"/>
       <c r="AF322" s="2"/>
     </row>
-    <row r="323" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="323" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A323" s="2"/>
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
@@ -14340,7 +14356,7 @@
       <c r="AE323" s="2"/>
       <c r="AF323" s="2"/>
     </row>
-    <row r="324" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="324" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A324" s="2"/>
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
@@ -14374,7 +14390,7 @@
       <c r="AE324" s="2"/>
       <c r="AF324" s="2"/>
     </row>
-    <row r="325" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="325" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A325" s="2"/>
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
@@ -14408,7 +14424,7 @@
       <c r="AE325" s="2"/>
       <c r="AF325" s="2"/>
     </row>
-    <row r="326" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="326" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A326" s="2"/>
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
@@ -14442,7 +14458,7 @@
       <c r="AE326" s="2"/>
       <c r="AF326" s="2"/>
     </row>
-    <row r="327" spans="1:32" x14ac:dyDescent="0.75">
+    <row r="327" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A327" s="2"/>
       <c r="B327" s="2"/>
       <c r="C327" s="2"/>

</xml_diff>

<commit_message>
Immagini giochi e change foto Maria
</commit_message>
<xml_diff>
--- a/esercizi.xlsx
+++ b/esercizi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\iomimuovoacasa.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4DA75B-EB73-4088-A1CE-A5C5B942AA40}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968EE791-E846-4297-B36E-E7C5EBE6194A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="535">
   <si>
     <t>cartella</t>
   </si>
@@ -1630,6 +1630,21 @@
   </si>
   <si>
     <t>AER_LOrologioSvizzero.pdf</t>
+  </si>
+  <si>
+    <t>equilibrista.png</t>
+  </si>
+  <si>
+    <t>cestastelle.png</t>
+  </si>
+  <si>
+    <t>moscacieca.png</t>
+  </si>
+  <si>
+    <t>orologiosvizzero.png</t>
+  </si>
+  <si>
+    <t>granchio.png</t>
   </si>
 </sst>
 </file>
@@ -2001,8 +2016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="123" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="123" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2982,7 +2997,9 @@
       <c r="G20" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>530</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
@@ -3030,7 +3047,9 @@
       <c r="G21" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>531</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -3078,7 +3097,9 @@
       <c r="G22" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2" t="s">
+        <v>532</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -3126,7 +3147,9 @@
       <c r="G23" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="H23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -3174,7 +3197,9 @@
       <c r="G24" s="2" t="s">
         <v>515</v>
       </c>
-      <c r="H24" s="2"/>
+      <c r="H24" s="2" t="s">
+        <v>531</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -3222,7 +3247,9 @@
       <c r="G25" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="H25" s="2"/>
+      <c r="H25" s="2" t="s">
+        <v>534</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -3270,7 +3297,9 @@
       <c r="G26" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="H26" s="2"/>
+      <c r="H26" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -3318,7 +3347,9 @@
       <c r="G27" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>533</v>
+      </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>

</xml_diff>